<commit_message>
update the alu&decoder of the 30+
(not include division)
rewrite decoder and alu
add hilo register
rewrite sign extend
</commit_message>
<xml_diff>
--- a/auxiliary documents/control_signal.xlsx
+++ b/auxiliary documents/control_signal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Courses\计组\ex\硬件综合设计\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\workspace\vivado\hardware_comp\hardware_comp.srcs\sources_1\auxiliary documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="14250" windowHeight="7620"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="14250" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="45">
   <si>
     <t>memtoreg</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>SLTIU</t>
+  </si>
+  <si>
+    <t>hilowrite</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +491,7 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -511,19 +514,22 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -563,13 +569,16 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -609,8 +618,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -650,8 +662,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -691,8 +706,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -732,13 +750,16 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="B8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -778,11 +799,14 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -822,11 +846,14 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -866,11 +893,14 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -910,11 +940,14 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -954,11 +987,14 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -998,19 +1034,22 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="N15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1050,11 +1089,14 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1094,11 +1136,14 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1127,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1138,11 +1183,14 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="N18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1171,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1182,19 +1230,22 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="N20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1234,11 +1285,14 @@
       <c r="M21">
         <v>0</v>
       </c>
-      <c r="N21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1278,11 +1332,14 @@
       <c r="M22">
         <v>0</v>
       </c>
-      <c r="N22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1322,11 +1379,14 @@
       <c r="M23">
         <v>0</v>
       </c>
-      <c r="N23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1366,11 +1426,14 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1410,11 +1473,14 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1454,63 +1520,138 @@
       <c r="M26">
         <v>0</v>
       </c>
-      <c r="N26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="N27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="N28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="N29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="N30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="O30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="B31" t="s">
         <v>36</v>
       </c>
-      <c r="N31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1538,9 +1679,6 @@
       <c r="I32">
         <v>1</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
       <c r="K32">
         <v>0</v>
       </c>
@@ -1550,11 +1688,14 @@
       <c r="M32">
         <v>0</v>
       </c>
-      <c r="N32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1582,9 +1723,6 @@
       <c r="I33">
         <v>1</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
@@ -1594,11 +1732,14 @@
       <c r="M33">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1626,9 +1767,6 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>0</v>
       </c>
@@ -1638,11 +1776,14 @@
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="N34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1670,9 +1811,6 @@
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
       <c r="K35">
         <v>0</v>
       </c>
@@ -1682,11 +1820,14 @@
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="N35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1714,9 +1855,6 @@
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
       <c r="K36">
         <v>0</v>
       </c>
@@ -1726,11 +1864,14 @@
       <c r="M36">
         <v>0</v>
       </c>
-      <c r="N36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1758,9 +1899,6 @@
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
       <c r="K37">
         <v>0</v>
       </c>
@@ -1770,11 +1908,14 @@
       <c r="M37">
         <v>0</v>
       </c>
-      <c r="N37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1802,9 +1943,6 @@
       <c r="I38">
         <v>1</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
       <c r="K38">
         <v>0</v>
       </c>
@@ -1814,11 +1952,14 @@
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="N38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1846,9 +1987,6 @@
       <c r="I39">
         <v>1</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
       <c r="K39">
         <v>0</v>
       </c>
@@ -1858,7 +1996,10 @@
       <c r="M39">
         <v>0</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cp0 registers and corresponding MF inst
establish the cp0 register and its datapath
MF instruction decoder
MF hazards datapath
verified with corresponding tests
</commit_message>
<xml_diff>
--- a/auxiliary documents/control_signal.xlsx
+++ b/auxiliary documents/control_signal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="14250" windowHeight="7620"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="14250" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="66">
   <si>
     <t>memtoreg</t>
   </si>
@@ -196,6 +196,33 @@
   </si>
   <si>
     <t>BGEZAL</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>LBU</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>LHU</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>cp0write</t>
   </si>
 </sst>
 </file>
@@ -514,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N53" sqref="A50:N53"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -528,7 +555,7 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -565,8 +592,11 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -609,13 +639,22 @@
       <c r="N2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="B3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -658,8 +697,14 @@
       <c r="N4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -702,8 +747,14 @@
       <c r="N5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -746,8 +797,14 @@
       <c r="N6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -790,13 +847,22 @@
       <c r="N7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="B8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -839,11 +905,14 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -886,11 +955,14 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -933,11 +1005,14 @@
       <c r="N11">
         <v>0</v>
       </c>
-      <c r="O11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -980,11 +1055,14 @@
       <c r="N12">
         <v>0</v>
       </c>
-      <c r="O12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1027,11 +1105,14 @@
       <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1074,19 +1155,22 @@
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="O14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="O15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1129,11 +1213,14 @@
       <c r="N16">
         <v>0</v>
       </c>
-      <c r="O16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1176,11 +1263,14 @@
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1223,11 +1313,14 @@
       <c r="N18">
         <v>0</v>
       </c>
-      <c r="O18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1270,19 +1363,22 @@
       <c r="N19">
         <v>0</v>
       </c>
-      <c r="O19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="O20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1325,11 +1421,14 @@
       <c r="N21">
         <v>0</v>
       </c>
-      <c r="O21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1372,11 +1471,14 @@
       <c r="N22">
         <v>0</v>
       </c>
-      <c r="O22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1419,11 +1521,14 @@
       <c r="N23">
         <v>0</v>
       </c>
-      <c r="O23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1466,11 +1571,14 @@
       <c r="N24">
         <v>0</v>
       </c>
-      <c r="O24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1513,11 +1621,14 @@
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="O25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1560,11 +1671,14 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1607,11 +1721,14 @@
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1654,41 +1771,44 @@
       <c r="N28">
         <v>0</v>
       </c>
-      <c r="O28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="O29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="O30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="B31" t="s">
         <v>36</v>
       </c>
-      <c r="O31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1731,11 +1851,14 @@
       <c r="N32">
         <v>0</v>
       </c>
-      <c r="O32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1778,11 +1901,14 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1825,11 +1951,14 @@
       <c r="N34">
         <v>0</v>
       </c>
-      <c r="O34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1872,11 +2001,14 @@
       <c r="N35">
         <v>0</v>
       </c>
-      <c r="O35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1919,11 +2051,14 @@
       <c r="N36">
         <v>0</v>
       </c>
-      <c r="O36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1966,11 +2101,14 @@
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2013,11 +2151,14 @@
       <c r="N38">
         <v>0</v>
       </c>
-      <c r="O38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2060,16 +2201,22 @@
       <c r="N39">
         <v>0</v>
       </c>
-      <c r="O39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="B40" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="P40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2112,8 +2259,14 @@
       <c r="N41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2156,8 +2309,14 @@
       <c r="N42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2200,8 +2359,14 @@
       <c r="N43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2244,8 +2409,14 @@
       <c r="N44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2288,8 +2459,14 @@
       <c r="N45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2332,8 +2509,14 @@
       <c r="N46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2376,8 +2559,14 @@
       <c r="N47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2420,13 +2609,22 @@
       <c r="N48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="B49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="P49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2469,8 +2667,14 @@
       <c r="N50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2513,8 +2717,14 @@
       <c r="N51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2557,8 +2767,14 @@
       <c r="N52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2600,6 +2816,420 @@
       </c>
       <c r="N53">
         <v>1</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="P54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>